<commit_message>
parser work correct, but bad fit
</commit_message>
<xml_diff>
--- a/DC/dffd.xlsx
+++ b/DC/dffd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hz vs overvoltage" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="total" sheetId="8" r:id="rId3"/>
     <sheet name="Лист3" sheetId="5" r:id="rId4"/>
     <sheet name="line" sheetId="2" r:id="rId5"/>
-    <sheet name="Лист2" sheetId="4" r:id="rId6"/>
+    <sheet name="E_band" sheetId="4" r:id="rId6"/>
     <sheet name="t_dead" sheetId="9" r:id="rId7"/>
     <sheet name="Лист4" sheetId="10" r:id="rId8"/>
     <sheet name="exp" sheetId="3" r:id="rId9"/>
@@ -206,6 +206,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -371,11 +372,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189331288"/>
-        <c:axId val="189331672"/>
+        <c:axId val="226287504"/>
+        <c:axId val="226288288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189331288"/>
+        <c:axId val="226287504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,12 +433,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189331672"/>
+        <c:crossAx val="226288288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189331672"/>
+        <c:axId val="226288288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +495,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189331288"/>
+        <c:crossAx val="226287504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -676,11 +677,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189871488"/>
-        <c:axId val="189871880"/>
+        <c:axId val="227367208"/>
+        <c:axId val="227367600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189871488"/>
+        <c:axId val="227367208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,12 +738,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189871880"/>
+        <c:crossAx val="227367600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189871880"/>
+        <c:axId val="227367600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +800,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189871488"/>
+        <c:crossAx val="227367208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1031,11 +1032,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189872664"/>
-        <c:axId val="147238248"/>
+        <c:axId val="227368384"/>
+        <c:axId val="227368776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189872664"/>
+        <c:axId val="227368384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,12 +1093,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147238248"/>
+        <c:crossAx val="227368776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147238248"/>
+        <c:axId val="227368776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1154,7 +1155,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189872664"/>
+        <c:crossAx val="227368384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1386,11 +1387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147237464"/>
-        <c:axId val="147237072"/>
+        <c:axId val="227369560"/>
+        <c:axId val="227369952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147237464"/>
+        <c:axId val="227369560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,12 +1448,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147237072"/>
+        <c:crossAx val="227369952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147237072"/>
+        <c:axId val="227369952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1510,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147237464"/>
+        <c:crossAx val="227369560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1691,11 +1692,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191141920"/>
-        <c:axId val="191142312"/>
+        <c:axId val="227370736"/>
+        <c:axId val="227371128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191141920"/>
+        <c:axId val="227370736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,12 +1753,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191142312"/>
+        <c:crossAx val="227371128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191142312"/>
+        <c:axId val="227371128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1815,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191141920"/>
+        <c:crossAx val="227370736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2506,11 +2507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189309592"/>
-        <c:axId val="190230064"/>
+        <c:axId val="226289072"/>
+        <c:axId val="226289464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189309592"/>
+        <c:axId val="226289072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,12 +2568,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190230064"/>
+        <c:crossAx val="226289464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190230064"/>
+        <c:axId val="226289464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2629,7 +2630,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189309592"/>
+        <c:crossAx val="226289072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2920,11 +2921,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189304200"/>
-        <c:axId val="189351480"/>
+        <c:axId val="229155616"/>
+        <c:axId val="229156008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189304200"/>
+        <c:axId val="229155616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2981,12 +2982,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189351480"/>
+        <c:crossAx val="229156008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189351480"/>
+        <c:axId val="229156008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3043,7 +3044,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189304200"/>
+        <c:crossAx val="229155616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3957,11 +3958,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147238640"/>
-        <c:axId val="147239032"/>
+        <c:axId val="229158360"/>
+        <c:axId val="229158752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147238640"/>
+        <c:axId val="229158360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4018,12 +4019,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147239032"/>
+        <c:crossAx val="229158752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147239032"/>
+        <c:axId val="229158752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4080,7 +4081,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147238640"/>
+        <c:crossAx val="229158360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4492,11 +4493,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189866000"/>
-        <c:axId val="189866392"/>
+        <c:axId val="229159536"/>
+        <c:axId val="229159928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189866000"/>
+        <c:axId val="229159536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4553,12 +4554,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189866392"/>
+        <c:crossAx val="229159928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189866392"/>
+        <c:axId val="229159928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4615,7 +4616,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189866000"/>
+        <c:crossAx val="229159536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4711,6 +4712,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4834,11 +4836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189867176"/>
-        <c:axId val="189867568"/>
+        <c:axId val="229161104"/>
+        <c:axId val="229161496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189867176"/>
+        <c:axId val="229161104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4895,12 +4897,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189867568"/>
+        <c:crossAx val="229161496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189867568"/>
+        <c:axId val="229161496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4957,7 +4959,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189867176"/>
+        <c:crossAx val="229161104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5021,6 +5023,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5133,11 +5136,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189868352"/>
-        <c:axId val="189868744"/>
+        <c:axId val="229162280"/>
+        <c:axId val="229162672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189868352"/>
+        <c:axId val="229162280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5194,12 +5197,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189868744"/>
+        <c:crossAx val="229162672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189868744"/>
+        <c:axId val="229162672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5256,7 +5259,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189868352"/>
+        <c:crossAx val="229162280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5320,6 +5323,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5486,11 +5490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189865608"/>
-        <c:axId val="189869528"/>
+        <c:axId val="229160712"/>
+        <c:axId val="229157968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189865608"/>
+        <c:axId val="229160712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5547,12 +5551,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189869528"/>
+        <c:crossAx val="229157968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189869528"/>
+        <c:axId val="229157968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5609,7 +5613,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189865608"/>
+        <c:crossAx val="229160712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5673,6 +5677,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5797,11 +5802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189870312"/>
-        <c:axId val="189870704"/>
+        <c:axId val="229157184"/>
+        <c:axId val="229156792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189870312"/>
+        <c:axId val="229157184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5858,12 +5863,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189870704"/>
+        <c:crossAx val="229156792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189870704"/>
+        <c:axId val="229156792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5920,7 +5925,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189870312"/>
+        <c:crossAx val="229157184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15275,8 +15280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15838,7 +15843,7 @@
   <dimension ref="A1:X79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17585,10 +17590,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17627,6 +17632,15 @@
         <v>1.1323499472751401E-2</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>D4*2*A2</f>
+        <v>0.80313518396000017</v>
+      </c>
+      <c r="D4">
+        <v>4660</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17637,7 +17651,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>